<commit_message>
Basic and Monte Carlo modes now working
</commit_message>
<xml_diff>
--- a/simconfig.xlsx
+++ b/simconfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="551" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Conditions (Weather)" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
   <si>
     <t>Total inert mass</t>
   </si>
@@ -57,33 +57,6 @@
     <t>Monte Carlo</t>
   </si>
   <si>
-    <t>Chamber pressure</t>
-  </si>
-  <si>
-    <t>psia</t>
-  </si>
-  <si>
-    <t>Expansion ratio</t>
-  </si>
-  <si>
-    <t>Engine mass</t>
-  </si>
-  <si>
-    <t>Contraction ratio</t>
-  </si>
-  <si>
-    <t>Characteristic length</t>
-  </si>
-  <si>
-    <t>Chamber-to-throat contraction angle</t>
-  </si>
-  <si>
-    <t>degrees</t>
-  </si>
-  <si>
-    <t>Nozzle cone half angle</t>
-  </si>
-  <si>
     <t>Ambient temperature</t>
   </si>
   <si>
@@ -96,27 +69,9 @@
     <t>Pa</t>
   </si>
   <si>
-    <t>Oxidizer</t>
-  </si>
-  <si>
-    <t>Fuel</t>
-  </si>
-  <si>
-    <t>NITROUSOXIDE</t>
-  </si>
-  <si>
-    <t>N2O</t>
-  </si>
-  <si>
-    <t>ETHANE</t>
-  </si>
-  <si>
     <t>Oxidizer volume</t>
   </si>
   <si>
-    <t>Propellant options</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -195,9 +150,6 @@
     <t>Fuel Mass</t>
   </si>
   <si>
-    <t>C2H6</t>
-  </si>
-  <si>
     <t>m^3</t>
   </si>
   <si>
@@ -213,9 +165,6 @@
     <t>Launch Altitude</t>
   </si>
   <si>
-    <t>Tank</t>
-  </si>
-  <si>
     <t>Tank Mass Calculation</t>
   </si>
   <si>
@@ -309,64 +258,16 @@
     <t>Truth of Consequences US Climate Data</t>
   </si>
   <si>
-    <t>Fuel Injector Area</t>
-  </si>
-  <si>
-    <t>m^2</t>
-  </si>
-  <si>
-    <t>Oxidizer Injector Area</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Oxidizer Valve Cv</t>
   </si>
   <si>
     <t>Fuel Valve Cv</t>
   </si>
   <si>
-    <t># of oxidizer injector elements</t>
-  </si>
-  <si>
-    <t>Oxidizer injector element area</t>
-  </si>
-  <si>
-    <t>Oxidizer injector element diameter</t>
-  </si>
-  <si>
-    <t># of fuel injector elements</t>
-  </si>
-  <si>
-    <t>Fuel injector element diameter</t>
-  </si>
-  <si>
-    <t>Fuel injector element area</t>
-  </si>
-  <si>
-    <t>Oxidizer Injector Cd</t>
-  </si>
-  <si>
-    <t>Fuel Injector Cd</t>
-  </si>
-  <si>
     <t>Fuel temperature</t>
   </si>
   <si>
     <t>Oxidizer temperature</t>
-  </si>
-  <si>
-    <t>Engine throat area</t>
-  </si>
-  <si>
-    <t>Throat area</t>
-  </si>
-  <si>
-    <t>in^2</t>
-  </si>
-  <si>
-    <t>C* efficiency</t>
   </si>
   <si>
     <t>Diameter</t>
@@ -442,12 +343,6 @@
     <t>Factor</t>
   </si>
   <si>
-    <t>Ignition Time</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>New Mass</t>
   </si>
   <si>
@@ -476,6 +371,18 @@
   </si>
   <si>
     <t>Receive Sensitivity</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>AeroTech_L1390</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +925,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G1" s="10" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1037,7 +944,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -1048,7 +955,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,7 +974,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>8</v>
@@ -1079,10 +986,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1101,7 +1008,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1112,7 +1019,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,7 +1038,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -1143,7 +1050,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1162,7 +1069,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -1189,7 +1096,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -1200,12 +1107,12 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
@@ -1228,7 +1135,7 @@
     </row>
     <row r="26" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
@@ -1239,10 +1146,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1261,7 +1168,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
@@ -1272,10 +1179,10 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1317,14 +1224,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1339,7 +1246,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G1" s="12" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="I1" t="str">
         <f>IF(H2="Single value","Value",IF(H2="Range of values","Start",IF(H2="Monte Carlo","Mean","ERROR")))</f>
@@ -1354,10 +1261,10 @@
         <v/>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="P1" t="str">
         <f>IF(O2="Single value","Value",IF(O2="Range of values","Start",IF(O2="Monte Carlo","Mean","ERROR")))</f>
@@ -1372,24 +1279,24 @@
         <v/>
       </c>
       <c r="S1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -1403,7 +1310,7 @@
         <v>3</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>8</v>
@@ -1419,7 +1326,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2">
         <f>I6*I7</f>
@@ -1429,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="E3">
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
@@ -1446,12 +1353,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2">
         <f>I14*I15</f>
@@ -1461,13 +1368,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="P4" t="str">
         <f>IF(O5="Single value","Value",IF(O5="Range of values","Start",IF(O5="Monte Carlo","Mean","ERROR")))</f>
@@ -1482,12 +1389,12 @@
         <v/>
       </c>
       <c r="S4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2">
         <v>0.5</v>
@@ -1496,13 +1403,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="E5">
         <v>0.5</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="I5" t="str">
         <f>IF(H6="Single value","Value",IF(H6="Range of values","Start",IF(H6="Monte Carlo","Mean","ERROR")))</f>
@@ -1517,10 +1424,10 @@
         <v/>
       </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>8</v>
@@ -1536,23 +1443,21 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2">
         <f>B13+B12+B11+B7</f>
-        <v>7.8248337773341383</v>
+        <v>5.8248337773341383</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>8</v>
@@ -1568,7 +1473,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <f>I10*I11</f>
@@ -1578,13 +1483,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>8</v>
@@ -1595,10 +1500,10 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="P7" t="str">
         <f>IF(O8="Single value","Value",IF(O8="Range of values","Start",IF(O8="Monte Carlo","Mean","ERROR")))</f>
@@ -1613,12 +1518,12 @@
         <v/>
       </c>
       <c r="S7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>2.5</v>
@@ -1627,13 +1532,13 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>8</v>
@@ -1645,12 +1550,12 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
@@ -1660,10 +1565,10 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>35.324833777334135</v>
+        <v>33.324833777334135</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I9" t="str">
         <f>IF(H10="Single value","Value",IF(H10="Range of values","Start",IF(H10="Monte Carlo","Mean","ERROR")))</f>
@@ -1678,10 +1583,10 @@
         <v/>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>8</v>
@@ -1693,22 +1598,21 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
-        <f>11.151/2.205</f>
-        <v>5.0571428571428569</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>8</v>
@@ -1722,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>8</v>
@@ -1733,7 +1637,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1741,14 +1645,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="2">
-        <f>I2*I3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>8</v>
@@ -1759,10 +1662,10 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>8</v>
@@ -1773,7 +1676,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1799,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="I13" t="str">
         <f>IF(H14="Single value","Value",IF(H14="Range of values","Start",IF(H14="Monte Carlo","Mean","ERROR")))</f>
@@ -1814,10 +1717,10 @@
         <v/>
       </c>
       <c r="L13" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="P13" t="str">
         <f>IF(O14="Single value","Value",IF(O14="Range of values","Start",IF(O14="Monte Carlo","Mean","ERROR")))</f>
@@ -1832,22 +1735,28 @@
         <v/>
       </c>
       <c r="S13" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2">
-        <f>'Propellant Parameters (Tanks)'!N26*0.453592</f>
-        <v>15.160295301298001</v>
+        <f>SUM(B3:B13)*E14</f>
+        <v>2.2237250666001205</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.15</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>8</v>
@@ -1858,10 +1767,10 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>8</v>
@@ -1876,24 +1785,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15">
-        <f>SUM(B3:B14)*E15</f>
-        <v>5.8563407903662492</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="31">
-        <v>0.15</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>8</v>
@@ -1904,10 +1797,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>8</v>
@@ -1918,24 +1811,24 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C30" t="str">
         <f>IF(B31="Single value","Value",IF(B31="Range of values","Start",IF(B31="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
+        <v>Mean</v>
       </c>
       <c r="D30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","Step",IF(B31="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
+        <v>Standard deviation</v>
       </c>
       <c r="E30" t="str">
         <f>IF(B31="Single value","",IF(B31="Range of values","End",IF(B31="Monte Carlo","","ERROR")))</f>
         <v/>
       </c>
       <c r="F30" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1943,13 +1836,14 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C31" s="3">
-        <f>SUM(B:B)</f>
-        <v>44.898612726141245</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" t="s">
         <v>3</v>
@@ -1957,7 +1851,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>6.125</v>
@@ -1994,7 +1888,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2017,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F59"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,544 +1923,34 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" t="str">
-        <f>IF(B3="Single value","Value",IF(B3="Range of values","Start",IF(B3="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(B3="Single value","",IF(B3="Range of values","Step",IF(B3="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <f>IF(B3="Single value","",IF(B3="Range of values","End",IF(B3="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>300</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" t="str">
-        <f>IF(B6="Single value","Value",IF(B6="Range of values","Start",IF(B6="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(B6="Single value","",IF(B6="Range of values","Step",IF(B6="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <f>IF(B6="Single value","",IF(B6="Range of values","End",IF(B6="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4.99</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="str">
-        <f>IF(B9="Single value","Value",IF(B9="Range of values","Start",IF(B9="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D8" t="str">
-        <f>IF(B9="Single value","",IF(B9="Range of values","Step",IF(B9="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E8" t="str">
-        <f>IF(B9="Single value","",IF(B9="Range of values","End",IF(B9="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="str">
-        <f>IF(B12="Single value","Value",IF(B12="Range of values","Start",IF(B12="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(B12="Single value","",IF(B12="Range of values","Step",IF(B12="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <f>IF(B12="Single value","",IF(B12="Range of values","End",IF(B12="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="str">
-        <f>IF(B15="Single value","Value",IF(B15="Range of values","Start",IF(B15="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D14" t="str">
-        <f>IF(B15="Single value","",IF(B15="Range of values","Step",IF(B15="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E14" t="str">
-        <f>IF(B15="Single value","",IF(B15="Range of values","End",IF(B15="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="str">
-        <f>IF(B18="Single value","Value",IF(B18="Range of values","Start",IF(B18="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(B18="Single value","",IF(B18="Range of values","Step",IF(B18="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <f>IF(B18="Single value","",IF(B18="Range of values","End",IF(B18="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C20" t="str">
-        <f>IF(B21="Single value","Value",IF(B21="Range of values","Start",IF(B21="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D20" t="str">
-        <f>IF(B21="Single value","",IF(B21="Range of values","Step",IF(B21="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E20" t="str">
-        <f>IF(B21="Single value","",IF(B21="Range of values","End",IF(B21="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="str">
-        <f>IF(B24="Single value","Value",IF(B24="Range of values","Start",IF(B24="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D23" t="str">
-        <f>IF(B24="Single value","",IF(B24="Range of values","Step",IF(B24="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E23" t="str">
-        <f>IF(B24="Single value","",IF(B24="Range of values","End",IF(B24="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>112</v>
       </c>
-      <c r="C26">
-        <v>1.4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C27" t="str">
-        <f>IF(B28="Single value","Value",IF(B28="Range of values","Start",IF(B28="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(B28="Single value","",IF(B28="Range of values","Step",IF(B28="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E27" t="str">
-        <f>IF(B28="Single value","",IF(B28="Range of values","End",IF(B28="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1">
-        <f>C26*2.54^2/100^2</f>
-        <v>9.03224E-4</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36">
-        <f>B35 * 2.54/100</f>
-        <v>6.3500000000000004E-4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37">
-        <f>(PI() / 4) *B36^2</f>
-        <v>3.1669217443593616E-7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>103</v>
-      </c>
-      <c r="B40">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41">
-        <f>B40 * 2.54/100</f>
-        <v>1.2953999999999999E-3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42">
-        <f>(PI() / 4) *B41^2</f>
-        <v>1.3179461531325915E-6</v>
-      </c>
-      <c r="C42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C44" t="str">
-        <f>IF(B45="Single value","Value",IF(B45="Range of values","Start",IF(B45="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D44" t="str">
-        <f>IF(B45="Single value","",IF(B45="Range of values","Step",IF(B45="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E44" t="str">
-        <f>IF(B45="Single value","",IF(B45="Range of values","End",IF(B45="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="9">
-        <f>B34*B37</f>
-        <v>1.5201224372924936E-5</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C47" t="str">
-        <f>IF(B48="Single value","Value",IF(B48="Range of values","Start",IF(B48="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D47" t="str">
-        <f>IF(B48="Single value","",IF(B48="Range of values","Step",IF(B48="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E47" t="str">
-        <f>IF(B48="Single value","",IF(B48="Range of values","End",IF(B48="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="9">
-        <f>B42*B39</f>
-        <v>3.1630707675182194E-5</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C50" t="str">
-        <f>IF(B51="Single value","Value",IF(B51="Range of values","Start",IF(B51="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D50" t="str">
-        <f>IF(B51="Single value","",IF(B51="Range of values","Step",IF(B51="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E50" t="str">
-        <f>IF(B51="Single value","",IF(B51="Range of values","End",IF(B51="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C53" t="str">
-        <f>IF(B54="Single value","Value",IF(B54="Range of values","Start",IF(B54="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D53" t="str">
-        <f>IF(B54="Single value","",IF(B54="Range of values","Step",IF(B54="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E53" t="str">
-        <f>IF(B54="Single value","",IF(B54="Range of values","End",IF(B54="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" t="str">
-        <f>IF(B59="Single value","Value",IF(B59="Range of values","Start",IF(B59="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D58" t="str">
-        <f>IF(B59="Single value","",IF(B59="Range of values","Step",IF(B59="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E58" t="str">
-        <f>IF(B59="Single value","",IF(B59="Range of values","End",IF(B59="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" t="s">
-        <v>136</v>
+      <c r="B2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Validation!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3 B6 B9 B12 B15 B18 B21 B24 B28 B59</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Validation!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B45 B48 B51 B54</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,126 +1963,153 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21" t="str">
+        <f>IF(B4="Single value","Value",IF(B4="Range of values","Start",IF(B4="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D3" s="21" t="str">
+        <f>IF(B4="Single value","",IF(B4="Range of values","Step",IF(B4="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E3" s="21" t="str">
+        <f>IF(B4="Single value","",IF(B4="Range of values","End",IF(B4="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="25">
+        <f>$N$4*J4</f>
+        <v>2.6219360000000001E-2</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1600</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
+      <c r="N4" s="6">
+        <v>1.6387100000000001E-5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21" t="str">
-        <f>IF(B7="Single value","Value",IF(B7="Range of values","Start",IF(B7="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D6" s="21" t="str">
-        <f>IF(B7="Single value","",IF(B7="Range of values","Step",IF(B7="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E6" s="21" t="str">
-        <f>IF(B7="Single value","",IF(B7="Range of values","End",IF(B7="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
+      <c r="A6" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="25">
+        <f>$N$4*J6</f>
+        <v>1.5076132000000001E-2</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="22" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="J6" s="1">
+        <v>920</v>
       </c>
       <c r="K6" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="25">
-        <f>$N$7*J7</f>
-        <v>2.6219360000000001E-2</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1600</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="6">
-        <v>1.6387100000000001E-5</v>
-      </c>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="C8" s="21" t="str">
+        <f>IF(B9="Single value","Value",IF(B9="Range of values","Start",IF(B9="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D8" s="21" t="str">
+        <f>IF(B9="Single value","",IF(B9="Range of values","Step",IF(B9="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E8" s="21" t="str">
+        <f>IF(B9="Single value","",IF(B9="Range of values","End",IF(B9="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
       <c r="F8" s="22"/>
+      <c r="J8" s="4">
+        <f>93.19</f>
+        <v>93.19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25">
-        <f>$N$7*J9</f>
-        <v>1.5076132000000001E-2</v>
+      <c r="C9" s="26">
+        <v>0.15</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="1">
-        <v>920</v>
-      </c>
-      <c r="K9" t="s">
         <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2708,87 +2119,87 @@
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="22"/>
+      <c r="J10" s="4">
+        <v>5.625</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>2.5399999999999999E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="str">
-        <f>IF(B12="Single value","Value",IF(B12="Range of values","Start",IF(B12="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D11" s="21" t="str">
-        <f>IF(B12="Single value","",IF(B12="Range of values","Step",IF(B12="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E11" s="21" t="str">
-        <f>IF(B12="Single value","",IF(B12="Range of values","End",IF(B12="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="J11" s="4">
-        <f>93.19</f>
-        <v>93.19</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="A11" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="22" t="s">
         <v>42</v>
       </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="26">
-        <v>0.15</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" t="s">
-        <v>131</v>
-      </c>
-      <c r="N12" t="s">
-        <v>60</v>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="J12" s="1">
+        <v>5.9089999999999998</v>
+      </c>
+      <c r="K12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="21" t="str">
+        <f>IF(B14="Single value","Value",IF(B14="Range of values","Start",IF(B14="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D13" s="21" t="str">
+        <f>IF(B14="Single value","",IF(B14="Range of values","Step",IF(B14="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E13" s="21" t="str">
+        <f>IF(B14="Single value","",IF(B14="Range of values","End",IF(B14="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
       <c r="F13" s="22"/>
-      <c r="J13" s="4">
-        <v>5.625</v>
-      </c>
-      <c r="K13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N13">
-        <v>2.5399999999999999E-2</v>
-      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="26">
-        <v>0.15</v>
+      <c r="C14" s="25">
+        <f>C4*(1-C9)</f>
+        <v>2.2286456E-2</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
       <c r="F14" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" t="s">
-        <v>131</v>
+        <v>42</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="K14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2798,285 +2209,261 @@
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="22"/>
-      <c r="J15" s="1">
-        <v>5.9089999999999998</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21" t="str">
-        <f>IF(B17="Single value","Value",IF(B17="Range of values","Start",IF(B17="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D16" s="21" t="str">
-        <f>IF(B17="Single value","",IF(B17="Range of values","Step",IF(B17="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E16" s="21" t="str">
-        <f>IF(B17="Single value","",IF(B17="Range of values","End",IF(B17="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="A16" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="29">
+        <f>C6*(1-C11)</f>
+        <v>1.28147122E-2</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="30" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="25">
-        <f>C7*(1-C12)</f>
-        <v>2.2286456E-2</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="22" t="s">
+      <c r="J17" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" t="str">
+        <f>IF(B19="Single value","Value",IF(B19="Range of values","Start",IF(B19="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(B19="Single value","",IF(B19="Range of values","Step",IF(B19="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <f>IF(B19="Single value","",IF(B19="Range of values","End",IF(B19="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="J18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="21"/>
+      <c r="J19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>2.52</v>
+      </c>
+      <c r="M19" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="13">
+        <f>K19*L19</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G20" s="6"/>
+      <c r="J20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="8">
+        <f>C45</f>
+        <v>64.385192990722629</v>
+      </c>
+      <c r="L20">
+        <v>0.249</v>
+      </c>
+      <c r="M20" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="13">
+        <f>K20*L20</f>
+        <v>16.031913054689934</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="9">
+        <f>$N$4*J8</f>
+        <v>1.5271138490000002E-3</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1"/>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="8">
+        <f>C48</f>
+        <v>37.02148596966552</v>
+      </c>
+      <c r="L21">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M21" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" s="13">
+        <f>K21*L21</f>
+        <v>10.069844183749023</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G22" s="6"/>
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="M22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N22">
+        <f>K22*L22</f>
+        <v>2.2810000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9">
+        <f>$N$10*J10</f>
+        <v>0.142875</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="1">
-        <v>0.28399999999999997</v>
-      </c>
-      <c r="K17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="29">
-        <f>C9*(1-C14)</f>
-        <v>1.28147122E-2</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J20" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" t="str">
-        <f>IF(B22="Single value","Value",IF(B22="Range of values","Start",IF(B22="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D21" t="str">
-        <f>IF(B22="Single value","",IF(B22="Range of values","Step",IF(B22="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E21" t="str">
-        <f>IF(B22="Single value","",IF(B22="Range of values","End",IF(B22="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" t="s">
-        <v>68</v>
-      </c>
-      <c r="L21" t="s">
-        <v>53</v>
-      </c>
-      <c r="M21" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="21"/>
-      <c r="J22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22">
-        <v>2</v>
-      </c>
-      <c r="L22">
-        <v>2.52</v>
-      </c>
-      <c r="M22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N22" s="13">
-        <f>K22*L22</f>
-        <v>5.04</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G23" s="6"/>
-      <c r="J23" t="s">
-        <v>71</v>
-      </c>
-      <c r="K23" s="8">
-        <f>C48</f>
-        <v>64.385192990722629</v>
-      </c>
-      <c r="L23">
-        <v>0.249</v>
-      </c>
-      <c r="M23" t="s">
-        <v>73</v>
-      </c>
-      <c r="N23" s="13">
-        <f>K23*L23</f>
-        <v>16.031913054689934</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="9">
-        <f>$N$7*J11</f>
-        <v>1.5271138490000002E-3</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="1"/>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="J24" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="8">
-        <f>C51</f>
-        <v>37.02148596966552</v>
-      </c>
-      <c r="L24">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="M24" t="s">
-        <v>73</v>
-      </c>
-      <c r="N24" s="13">
-        <f>K24*L24</f>
-        <v>10.069844183749023</v>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="14">
+        <f>SUM(N19:N22)</f>
+        <v>33.422757238438955</v>
+      </c>
+      <c r="O23" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G25" s="6"/>
-      <c r="J25" t="s">
-        <v>74</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>2.2810000000000001</v>
-      </c>
-      <c r="M25" t="s">
-        <v>69</v>
-      </c>
-      <c r="N25">
-        <f>K25*L25</f>
-        <v>2.2810000000000001</v>
+      <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="9">
+        <f>$N$10*J12</f>
+        <v>0.15008859999999999</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="9">
-        <f>$N$13*J13</f>
-        <v>0.142875</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" t="s">
-        <v>31</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="14">
-        <f>SUM(N22:N25)</f>
-        <v>33.422757238438955</v>
-      </c>
-      <c r="O26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="9">
-        <f>$N$13*J15</f>
-        <v>0.15008859999999999</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" t="s">
-        <v>31</v>
+      <c r="J26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9">
+        <f>$N$10*J14</f>
+        <v>7.2135999999999988E-3</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J29" t="s">
-        <v>116</v>
+      <c r="C29" t="str">
+        <f>IF(B30="Single value","Value",IF(B30="Range of values","Start",IF(B30="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(B30="Single value","",IF(B30="Range of values","Step",IF(B30="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <f>IF(B30="Single value","",IF(B30="Range of values","End",IF(B30="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="9">
-        <f>$N$13*J17</f>
-        <v>7.2135999999999988E-3</v>
+      <c r="C30" s="1">
+        <v>290</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3095,7 +2482,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>8</v>
@@ -3106,37 +2493,41 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C35" t="str">
-        <f>IF(B36="Single value","Value",IF(B36="Range of values","Start",IF(B36="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D35" t="str">
-        <f>IF(B36="Single value","",IF(B36="Range of values","Step",IF(B36="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E35" t="str">
-        <f>IF(B36="Single value","",IF(B36="Range of values","End",IF(B36="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1">
-        <v>290</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="str">
+        <f>IF(B38="Single value","Value",IF(B38="Range of values","Start",IF(B38="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(B38="Single value","",IF(B38="Range of values","Step",IF(B38="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <f>IF(B38="Single value","",IF(B38="Range of values","End",IF(B38="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1">
+        <f>G38/F38</f>
+        <v>24</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3155,14 +2546,14 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="1">
         <f>G41/F41</f>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -3170,51 +2561,51 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" t="str">
-        <f>IF(B44="Single value","Value",IF(B44="Range of values","Start",IF(B44="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D43" t="str">
-        <f>IF(B44="Single value","",IF(B44="Range of values","Step",IF(B44="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E43" t="str">
-        <f>IF(B44="Single value","",IF(B44="Range of values","End",IF(B44="Monte Carlo","","ERROR")))</f>
-        <v/>
+      <c r="A43" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="1">
-        <f>G44/F44</f>
-        <v>6</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>44</v>
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="str">
+        <f>IF(B45="Single value","Value",IF(B45="Range of values","Start",IF(B45="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(B45="Single value","",IF(B45="Range of values","Step",IF(B45="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <f>IF(B45="Single value","",IF(B45="Range of values","End",IF(B45="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="8">
+        <f>C4/((PI()/4)*C23^2)/N10</f>
+        <v>64.385192990722629</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C47" t="str">
         <f>IF(B48="Single value","Value",IF(B48="Range of values","Start",IF(B48="Monte Carlo","Mean","ERROR")))</f>
@@ -3231,120 +2622,93 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="8">
-        <f>C7/((PI()/4)*C26^2)/N13</f>
-        <v>64.385192990722629</v>
+        <f>C6/((PI()/4)*C23^2)/N10</f>
+        <v>37.02148596966552</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="str">
+        <f>IF(B50="Single value","Value",IF(B50="Range of values","Start",IF(B50="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D49" t="str">
+        <f>IF(B50="Single value","",IF(B50="Range of values","Step",IF(B50="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <f>IF(B50="Single value","",IF(B50="Range of values","End",IF(B50="Monte Carlo","","ERROR")))</f>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" t="str">
-        <f>IF(B51="Single value","Value",IF(B51="Range of values","Start",IF(B51="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D50" t="str">
-        <f>IF(B51="Single value","",IF(B51="Range of values","Step",IF(B51="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E50" t="str">
-        <f>IF(B51="Single value","",IF(B51="Range of values","End",IF(B51="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="8">
-        <f>C9/((PI()/4)*C26^2)/N13</f>
-        <v>37.02148596966552</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C52" t="str">
-        <f>IF(B53="Single value","Value",IF(B53="Range of values","Start",IF(B53="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D52" t="str">
-        <f>IF(B53="Single value","",IF(B53="Range of values","Step",IF(B53="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E52" t="str">
-        <f>IF(B53="Single value","",IF(B53="Range of values","End",IF(B53="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="7">
+      <c r="A50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="7">
         <f>41.668101-2</f>
         <v>39.668101</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D50" s="4">
         <v>0.25</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E50" s="7">
         <f>41.668101+2</f>
         <v>43.668101</v>
       </c>
-      <c r="F53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="str">
-        <f>IF(B55="Single value","Value",IF(B55="Range of values","Start",IF(B55="Monte Carlo","Mean","ERROR")))</f>
-        <v>Value</v>
-      </c>
-      <c r="D54" t="str">
-        <f>IF(B55="Single value","",IF(B55="Range of values","Step",IF(B55="Monte Carlo","Standard deviation","ERROR")))</f>
-        <v/>
-      </c>
-      <c r="E54" t="str">
-        <f>IF(B55="Single value","",IF(B55="Range of values","End",IF(B55="Monte Carlo","","ERROR")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="7">
+      <c r="F50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="str">
+        <f>IF(B52="Single value","Value",IF(B52="Range of values","Start",IF(B52="Monte Carlo","Mean","ERROR")))</f>
+        <v>Value</v>
+      </c>
+      <c r="D51" t="str">
+        <f>IF(B52="Single value","",IF(B52="Range of values","Step",IF(B52="Monte Carlo","Standard deviation","ERROR")))</f>
+        <v/>
+      </c>
+      <c r="E51" t="str">
+        <f>IF(B52="Single value","",IF(B52="Range of values","End",IF(B52="Monte Carlo","","ERROR")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="7">
         <v>5.0911735</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="1"/>
-      <c r="F55" t="s">
-        <v>48</v>
-      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="1"/>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
@@ -3353,51 +2717,44 @@
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
     </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="16"/>
+    </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
-      <c r="C59" s="17"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
       <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="19"/>
       <c r="E60" s="16"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
       <c r="E61" s="16"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="16"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3408,7 +2765,7 @@
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B7 B30:B31 B24 B26 B53 B28 B63 B61 B48 B51 B55:B56 B59 B33:B34 B17 B19 B9:B10 B12 B14:B15 B22 B36:B38 B41 B44</xm:sqref>
+          <xm:sqref>B4 B27:B28 B21 B23 B50 B25 B60 B58 B45 B48 B52:B53 B56 B30:B31 B14 B16 B6:B7 B9 B11:B12 B19 B33:B35 B38 B41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3446,7 +2803,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -3457,7 +2814,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3476,7 +2833,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -3487,7 +2844,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3506,7 +2863,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -3517,7 +2874,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3536,7 +2893,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -3547,7 +2904,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>